<commit_message>
Rebuilt mirror and housing, water proof
</commit_message>
<xml_diff>
--- a/modularRICH.xlsx
+++ b/modularRICH.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>parameter</t>
   </si>
@@ -96,12 +96,75 @@
   </si>
   <si>
     <t>mirrorSuppourtWidth</t>
+  </si>
+  <si>
+    <t>backGrooveBit</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>number 12</t>
+  </si>
+  <si>
+    <t>sensorHolderWidth</t>
+  </si>
+  <si>
+    <t>sensorHolderHeight</t>
+  </si>
+  <si>
+    <t>sensorHolderSensorWidth</t>
+  </si>
+  <si>
+    <t>sensorHolderSensorHeight</t>
+  </si>
+  <si>
+    <t>sensorHolderFlushORingID</t>
+  </si>
+  <si>
+    <t>12in Dash no. 274</t>
+  </si>
+  <si>
+    <t>frontBackORingID</t>
+  </si>
+  <si>
+    <t>15in Dash no. 281</t>
+  </si>
+  <si>
+    <t>oRingWidth</t>
+  </si>
+  <si>
+    <t>sensorHolderORingID</t>
+  </si>
+  <si>
+    <t>08in Dash no. 274</t>
+  </si>
+  <si>
+    <t>backMirrorGroove</t>
+  </si>
+  <si>
+    <t>mirrorGroove</t>
+  </si>
+  <si>
+    <t>compressionPercent</t>
+  </si>
+  <si>
+    <t>30-40 reccomended</t>
+  </si>
+  <si>
+    <t>fresnelChamfer</t>
+  </si>
+  <si>
+    <t>mirrorGrooveMill</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,8 +194,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,33 +477,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <f>0.25</f>
         <v>0.25</v>
       </c>
@@ -447,77 +516,77 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>100</v>
+      <c r="B4" s="1">
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>100</v>
+      <c r="B5" s="1">
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>100</v>
+      <c r="B6" s="1">
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>17</v>
+      <c r="B7" s="1">
+        <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>52</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <f>B8</f>
         <v>52</v>
       </c>
@@ -525,103 +594,272 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>0.1</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>100</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13">
-        <v>76.2</v>
+      <c r="B13" s="1">
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>1.49</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>0.06</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>90</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>3</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.189</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2.125</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2.125</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="1">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>40</v>
       </c>
-      <c r="C18" t="s">
-        <v>6</v>
+      <c r="B30" s="1">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added sensor, larger opening
</commit_message>
<xml_diff>
--- a/modularRICH.xlsx
+++ b/modularRICH.xlsx
@@ -107,12 +107,6 @@
     <t>number 12</t>
   </si>
   <si>
-    <t>sensorHolderWidth</t>
-  </si>
-  <si>
-    <t>sensorHolderHeight</t>
-  </si>
-  <si>
     <t>sensorHolderSensorWidth</t>
   </si>
   <si>
@@ -152,10 +146,16 @@
     <t>30-40 reccomended</t>
   </si>
   <si>
-    <t>fresnelChamfer</t>
-  </si>
-  <si>
     <t>mirrorGrooveMill</t>
+  </si>
+  <si>
+    <t>fresnelMirrorChamfer</t>
+  </si>
+  <si>
+    <t>detectorOpeningWidth</t>
+  </si>
+  <si>
+    <t>detectorOpeningHeight</t>
   </si>
 </sst>
 </file>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,7 +587,6 @@
         <v>13</v>
       </c>
       <c r="B9" s="1">
-        <f>B8</f>
         <v>52</v>
       </c>
       <c r="C9" t="s">
@@ -709,10 +708,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B20" s="1">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -720,10 +719,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -731,7 +730,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1">
         <v>2.125</v>
@@ -742,7 +741,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1">
         <v>2.125</v>
@@ -753,7 +752,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B24" s="1">
         <v>0.125</v>
@@ -764,7 +763,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B25" s="1">
         <v>8</v>
@@ -773,26 +772,26 @@
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B27" s="1">
         <v>16.5</v>
@@ -801,12 +800,12 @@
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1">
         <v>0.75</v>
@@ -817,7 +816,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B29" s="1">
         <v>0.25</v>
@@ -828,7 +827,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B30" s="1">
         <v>40</v>
@@ -837,12 +836,12 @@
         <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" s="1">
         <v>0.25</v>
@@ -853,7 +852,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B32" s="1">
         <v>0.125</v>

</xml_diff>

<commit_message>
Removed O-Rings 3cm aerogel, larger screws
</commit_message>
<xml_diff>
--- a/modularRICH.xlsx
+++ b/modularRICH.xlsx
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +509,6 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <f>0.25</f>
         <v>0.25</v>
       </c>
       <c r="C2" t="s">
@@ -521,7 +520,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -554,7 +553,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -598,10 +597,10 @@
         <v>14</v>
       </c>
       <c r="B10" s="1">
-        <v>3</v>
+        <v>0.125</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Top opening, parts have movable frames
</commit_message>
<xml_diff>
--- a/modularRICH.xlsx
+++ b/modularRICH.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>parameter</t>
   </si>
@@ -35,9 +35,6 @@
     <t>unit</t>
   </si>
   <si>
-    <t>acrylicThickness</t>
-  </si>
-  <si>
     <t>in</t>
   </si>
   <si>
@@ -95,67 +92,25 @@
     <t>fresnelEffectiveDiameter</t>
   </si>
   <si>
-    <t>mirrorSuppourtWidth</t>
-  </si>
-  <si>
-    <t>backGrooveBit</t>
-  </si>
-  <si>
     <t>note</t>
   </si>
   <si>
-    <t>number 12</t>
-  </si>
-  <si>
-    <t>sensorHolderSensorWidth</t>
-  </si>
-  <si>
-    <t>sensorHolderSensorHeight</t>
-  </si>
-  <si>
-    <t>sensorHolderFlushORingID</t>
-  </si>
-  <si>
-    <t>12in Dash no. 274</t>
-  </si>
-  <si>
-    <t>frontBackORingID</t>
-  </si>
-  <si>
-    <t>15in Dash no. 281</t>
-  </si>
-  <si>
     <t>oRingWidth</t>
   </si>
   <si>
-    <t>sensorHolderORingID</t>
-  </si>
-  <si>
-    <t>08in Dash no. 274</t>
-  </si>
-  <si>
-    <t>backMirrorGroove</t>
-  </si>
-  <si>
-    <t>mirrorGroove</t>
-  </si>
-  <si>
-    <t>compressionPercent</t>
-  </si>
-  <si>
-    <t>30-40 reccomended</t>
-  </si>
-  <si>
-    <t>mirrorGrooveMill</t>
-  </si>
-  <si>
-    <t>fresnelMirrorChamfer</t>
-  </si>
-  <si>
-    <t>detectorOpeningWidth</t>
-  </si>
-  <si>
-    <t>detectorOpeningHeight</t>
+    <t>sensorHolderDepth</t>
+  </si>
+  <si>
+    <t>frameAcrylicThickness</t>
+  </si>
+  <si>
+    <t>aerogelWidth</t>
+  </si>
+  <si>
+    <t>aerogelHeight</t>
+  </si>
+  <si>
+    <t>internalAcrylicThickness</t>
   </si>
 </sst>
 </file>
@@ -477,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,150 +456,150 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1">
-        <v>30</v>
+        <v>0.25</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>0.125</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1">
-        <v>0.1</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1">
-        <v>3</v>
+        <v>0.125</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
-        <v>1.49</v>
+        <v>0.1</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -652,212 +607,87 @@
         <v>20</v>
       </c>
       <c r="B15" s="1">
-        <v>0.06</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B18" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
         <v>90</v>
       </c>
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="1">
-        <v>3</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B21" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="1">
-        <v>0.189</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="1">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="1">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
       <c r="B22" s="1">
-        <v>2.125</v>
+        <v>0.75</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="1">
-        <v>2.125</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0.125</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="1">
-        <v>8</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="1">
-        <v>12</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="1">
-        <v>16.5</v>
-      </c>
-      <c r="C27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="1">
-        <v>40</v>
-      </c>
-      <c r="C30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="1">
-        <v>0.125</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rebuilt Modular RICH using submodules and reorganised directory structure
</commit_message>
<xml_diff>
--- a/modularRICH.xlsx
+++ b/modularRICH.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\OneDrive\projects\modularRICH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawai\OneDrive\projects\modularRICH\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>parameter</t>
   </si>
@@ -129,15 +129,6 @@
   </si>
   <si>
     <t>moduleSlotClearence</t>
-  </si>
-  <si>
-    <t>testMountLength</t>
-  </si>
-  <si>
-    <t>testMountWidth</t>
-  </si>
-  <si>
-    <t>testMountHeight</t>
   </si>
 </sst>
 </file>
@@ -460,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,39 +778,6 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="1">
-        <v>500</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="1">
-        <v>300</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="1">
-        <v>300</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Starting protoype of new design. First modifications after beamtest
</commit_message>
<xml_diff>
--- a/modularRICH.xlsx
+++ b/modularRICH.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawai\OneDrive\projects\modularRICH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\oneDrive\projects\modularRICH\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>parameter</t>
   </si>
@@ -59,12 +59,6 @@
     <t>deg</t>
   </si>
   <si>
-    <t>detectorWidth</t>
-  </si>
-  <si>
-    <t>detectorHeight</t>
-  </si>
-  <si>
     <t>mirrorThickness</t>
   </si>
   <si>
@@ -95,46 +89,22 @@
     <t>note</t>
   </si>
   <si>
-    <t>oRingWidth</t>
-  </si>
-  <si>
-    <t>sensorHolderDepth</t>
-  </si>
-  <si>
-    <t>frameAcrylicThickness</t>
-  </si>
-  <si>
     <t>aerogelWidth</t>
   </si>
   <si>
     <t>aerogelHeight</t>
   </si>
   <si>
-    <t>internalAcrylicThickness</t>
-  </si>
-  <si>
-    <t>aerogelClearence</t>
-  </si>
-  <si>
-    <t>backplanePCBWidth</t>
-  </si>
-  <si>
-    <t>backplanePCBHeight</t>
-  </si>
-  <si>
-    <t>backplaneHoleOffsett</t>
-  </si>
-  <si>
-    <t>backplanePostionOffsett</t>
-  </si>
-  <si>
-    <t>moduleSlotClearence</t>
+    <t>plasticThickness</t>
+  </si>
+  <si>
+    <t>aerogelHolderDepth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -167,10 +137,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,15 +444,15 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1">
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -491,21 +460,21 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>0.25</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -513,7 +482,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1">
         <v>110</v>
@@ -524,13 +493,14 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
-        <v>110</v>
+        <f>1.5-(1/32)</f>
+        <v>1.46875</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -560,8 +530,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <f>11.5-2*B2</f>
-        <v>10.75</v>
+        <v>5.75</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -583,10 +552,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="1">
-        <v>52</v>
+        <v>0.125</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -594,7 +563,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>52</v>
+        <v>0.1</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -602,13 +571,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
         <v>13</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0.125</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -616,167 +585,55 @@
         <v>14</v>
       </c>
       <c r="B14" s="1">
-        <v>0.1</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1">
-        <v>100</v>
+        <v>1.49</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
       <c r="B17" s="1">
-        <v>1.49</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="1">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>90</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1">
-        <v>6</v>
-      </c>
-      <c r="C20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="1">
-        <v>6.25E-2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="C22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0.125</v>
-      </c>
-      <c r="C23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="1">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="1">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="1">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Aluminium construction, new pcb backplane with MPPC array
</commit_message>
<xml_diff>
--- a/modularRICH.xlsx
+++ b/modularRICH.xlsx
@@ -95,10 +95,10 @@
     <t>aerogelHeight</t>
   </si>
   <si>
-    <t>plasticThickness</t>
-  </si>
-  <si>
     <t>aerogelHolderDepth</t>
+  </si>
+  <si>
+    <t>caseThickness</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +449,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1">
         <v>0.25</v>
@@ -493,7 +493,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1">
         <f>1.5-(1/32)</f>
@@ -530,7 +530,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>5.75</v>
+        <v>4.7300000000000004</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -637,5 +637,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Spacer resides with backplane
</commit_message>
<xml_diff>
--- a/modularRICH.xlsx
+++ b/modularRICH.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\oneDrive\projects\modularRICH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\oneDrive\projects\modularRICH\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -116,7 +116,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -150,7 +150,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,7 +434,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,8 +530,8 @@
         <v>23</v>
       </c>
       <c r="B8" s="2">
-        <f>1.5-(1/32)</f>
-        <v>1.46875</v>
+        <f>1.5-(1/16)</f>
+        <v>1.4375</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -564,7 +564,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>4.7300000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Made length longer, using 6 in fresnel
</commit_message>
<xml_diff>
--- a/modularRICH.xlsx
+++ b/modularRICH.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\oneDrive\projects\modularRICH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\oneDrive\projects\modularRICH\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -244,6 +244,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -279,6 +296,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -434,7 +468,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +642,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="2">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -619,7 +653,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
6in focal length, prep for drawings
</commit_message>
<xml_diff>
--- a/modularRICH.xlsx
+++ b/modularRICH.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\oneDrive\projects\modularRICH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\OneDrive\projects\modularRICH\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +598,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>4.5</v>
+        <v>7.5</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Mirror angle 2.5deg, front clamp added,larger aerogel area, depth 8in
</commit_message>
<xml_diff>
--- a/modularRICH.xlsx
+++ b/modularRICH.xlsx
@@ -468,7 +468,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,8 +564,8 @@
         <v>23</v>
       </c>
       <c r="B8" s="2">
-        <f>1.5-(1/16)</f>
-        <v>1.4375</v>
+        <f>2-(1/16)</f>
+        <v>1.9375</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -598,7 +598,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -609,7 +609,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="2">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Added four screws on front, incresed fresnel groove width to 70 thou
</commit_message>
<xml_diff>
--- a/modularRICH.xlsx
+++ b/modularRICH.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\oneDrive\projects\modularRICH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\OneDrive\projects\modularRICH\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>parameter</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>frontPanelThickness</t>
+  </si>
+  <si>
+    <t>fresnelGrooveWidth</t>
   </si>
 </sst>
 </file>
@@ -465,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,8 +567,8 @@
         <v>23</v>
       </c>
       <c r="B8" s="2">
-        <f>2-(1/16)</f>
-        <v>1.9375</v>
+        <f>2-B21</f>
+        <v>1.93</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -705,13 +708,24 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B22" s="1">
         <f>1/16</f>
         <v>6.25E-2</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed lens and holder and box shape
</commit_message>
<xml_diff>
--- a/modularRICH.xlsx
+++ b/modularRICH.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>parameter</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>fresnelGrooveWidth</t>
+  </si>
+  <si>
+    <t>lensMountThickness</t>
+  </si>
+  <si>
+    <t>lensDiameter</t>
+  </si>
+  <si>
+    <t>lensInsetDepth</t>
+  </si>
+  <si>
+    <t>lensCenterThickness</t>
   </si>
 </sst>
 </file>
@@ -468,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,8 +579,8 @@
         <v>23</v>
       </c>
       <c r="B8" s="2">
-        <f>2-B21</f>
-        <v>1.93</v>
+        <f>2.3-B26-(B23-B25)</f>
+        <v>1.505709</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -601,7 +613,8 @@
         <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>8</v>
+        <f>B16+(B26-(B23-B25))+B8+B21+1.5*B4</f>
+        <v>9.7469400000000004</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -656,7 +669,8 @@
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <v>6</v>
+        <f>7.44094-(B23-B25)</f>
+        <v>7.3159400000000003</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -711,7 +725,8 @@
         <v>28</v>
       </c>
       <c r="B21" s="1">
-        <v>7.0000000000000007E-2</v>
+        <f>B23</f>
+        <v>0.375</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
@@ -726,6 +741,50 @@
         <v>6.25E-2</v>
       </c>
       <c r="C22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.66929099999999997</v>
+      </c>
+      <c r="C26" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>